<commit_message>
add Load Board from DB
</commit_message>
<xml_diff>
--- a/docs/db_info/monopoly eav.xlsx
+++ b/docs/db_info/monopoly eav.xlsx
@@ -12,11 +12,12 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="62">
   <si>
     <t>OBJTYPE</t>
   </si>
@@ -99,9 +100,6 @@
     <t>WebIO</t>
   </si>
   <si>
-    <t>event</t>
-  </si>
-  <si>
     <t>doublesCount</t>
   </si>
   <si>
@@ -202,13 +200,16 @@
   </si>
   <si>
     <t>---------</t>
+  </si>
+  <si>
+    <t>---</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,6 +232,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -335,23 +343,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -363,11 +362,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -671,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,104 +710,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="G1" s="8" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="10"/>
-      <c r="M1" s="3" t="s">
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="9"/>
+      <c r="M1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="S1" s="5" t="s">
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="S1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="7"/>
-      <c r="X1" s="11" t="s">
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="13"/>
+      <c r="X1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="X2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Y2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="Z2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -812,21 +821,21 @@
       <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="4">
         <v>1</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="4">
         <f>A4</f>
         <v>2</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="4">
         <f>A5</f>
         <v>4</v>
       </c>
-      <c r="J3" t="s">
-        <v>59</v>
-      </c>
-      <c r="K3" t="str">
+      <c r="J3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="4" t="str">
         <f>J3</f>
         <v>currentPlayer_ref</v>
       </c>
@@ -845,19 +854,21 @@
       <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="G4">
+      <c r="F4" s="3"/>
+      <c r="G4" s="5">
         <v>2</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="5">
         <f>A8</f>
         <v>6</v>
       </c>
-      <c r="J4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" t="str">
+      <c r="I4" s="5"/>
+      <c r="J4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="5" t="str">
         <f>J4</f>
-        <v>event</v>
+        <v>position</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
@@ -882,10 +893,10 @@
         <v>4</v>
       </c>
       <c r="J5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" ref="K5:K41" si="0">J5</f>
+        <f t="shared" ref="K5:K40" si="0">J5</f>
         <v>doublesCount</v>
       </c>
     </row>
@@ -911,7 +922,7 @@
         <v>4</v>
       </c>
       <c r="J6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="0"/>
@@ -940,7 +951,7 @@
         <v>4</v>
       </c>
       <c r="J7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
@@ -961,17 +972,18 @@
       <c r="D8" t="s">
         <v>22</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="4">
         <v>6</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="4">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="J8" t="s">
-        <v>31</v>
-      </c>
-      <c r="K8" t="str">
+      <c r="I8" s="4"/>
+      <c r="J8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" s="4" t="str">
         <f t="shared" si="0"/>
         <v>name</v>
       </c>
@@ -994,7 +1006,7 @@
         <v>4</v>
       </c>
       <c r="J9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="0"/>
@@ -1010,7 +1022,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>
@@ -1023,7 +1035,7 @@
         <v>4</v>
       </c>
       <c r="J10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="0"/>
@@ -1052,7 +1064,7 @@
         <v>4</v>
       </c>
       <c r="J11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="0"/>
@@ -1086,7 +1098,7 @@
         <v>3</v>
       </c>
       <c r="J12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="0"/>
@@ -1102,7 +1114,7 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D13" t="str">
         <f>C13</f>
@@ -1116,7 +1128,7 @@
         <v>4</v>
       </c>
       <c r="J13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="0"/>
@@ -1132,7 +1144,7 @@
         <v>4</v>
       </c>
       <c r="J14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="0"/>
@@ -1148,7 +1160,7 @@
         <v>3</v>
       </c>
       <c r="J15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="0"/>
@@ -1164,7 +1176,7 @@
         <v>3</v>
       </c>
       <c r="J16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="0"/>
@@ -1172,17 +1184,18 @@
       </c>
     </row>
     <row r="17" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G17">
+      <c r="G17" s="4">
         <v>15</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="4">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J17" t="s">
-        <v>40</v>
-      </c>
-      <c r="K17" t="str">
+      <c r="I17" s="4"/>
+      <c r="J17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K17" s="4" t="str">
         <f t="shared" si="0"/>
         <v>description</v>
       </c>
@@ -1196,7 +1209,7 @@
         <v>3</v>
       </c>
       <c r="J18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K18" t="str">
         <f t="shared" si="0"/>
@@ -1212,7 +1225,7 @@
         <v>3</v>
       </c>
       <c r="J19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K19" t="str">
         <f t="shared" si="0"/>
@@ -1220,17 +1233,18 @@
       </c>
     </row>
     <row r="20" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G20">
+      <c r="G20" s="4">
         <v>18</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="4">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J20" t="s">
-        <v>31</v>
-      </c>
-      <c r="K20" t="str">
+      <c r="I20" s="4"/>
+      <c r="J20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K20" s="4" t="str">
         <f t="shared" si="0"/>
         <v>name</v>
       </c>
@@ -1244,7 +1258,7 @@
         <v>3</v>
       </c>
       <c r="J21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" si="0"/>
@@ -1260,7 +1274,7 @@
         <v>3</v>
       </c>
       <c r="J22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K22" t="str">
         <f t="shared" si="0"/>
@@ -1276,7 +1290,7 @@
         <v>3</v>
       </c>
       <c r="J23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K23" t="str">
         <f t="shared" si="0"/>
@@ -1292,7 +1306,7 @@
         <v>3</v>
       </c>
       <c r="J24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K24" t="str">
         <f t="shared" si="0"/>
@@ -1308,7 +1322,7 @@
         <v>3</v>
       </c>
       <c r="J25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K25" t="str">
         <f t="shared" si="0"/>
@@ -1320,11 +1334,11 @@
         <v>24</v>
       </c>
       <c r="H26">
-        <f>$A$7</f>
+        <f t="shared" ref="H26:H31" si="3">$A$7</f>
         <v>5</v>
       </c>
       <c r="J26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" si="0"/>
@@ -1336,29 +1350,30 @@
         <v>25</v>
       </c>
       <c r="H27">
-        <f t="shared" ref="H27:H31" si="3">$A$7</f>
-        <v>5</v>
-      </c>
-      <c r="J27" t="s">
-        <v>47</v>
-      </c>
-      <c r="K27" t="str">
-        <f t="shared" si="0"/>
-        <v>currentPrice</v>
-      </c>
-    </row>
-    <row r="28" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G28">
-        <v>26</v>
-      </c>
-      <c r="H28">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="J28" t="s">
-        <v>40</v>
-      </c>
-      <c r="K28" t="str">
+      <c r="J27" t="s">
+        <v>46</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="0"/>
+        <v>currentPrice</v>
+      </c>
+    </row>
+    <row r="28" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G28" s="4">
+        <v>26</v>
+      </c>
+      <c r="H28" s="4">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K28" s="4" t="str">
         <f t="shared" si="0"/>
         <v>description</v>
       </c>
@@ -1372,7 +1387,7 @@
         <v>5</v>
       </c>
       <c r="J29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K29" t="str">
         <f t="shared" si="0"/>
@@ -1380,17 +1395,18 @@
       </c>
     </row>
     <row r="30" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G30">
+      <c r="G30" s="4">
         <v>28</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="4">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="J30" t="s">
-        <v>31</v>
-      </c>
-      <c r="K30" t="str">
+      <c r="I30" s="4"/>
+      <c r="J30" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K30" s="4" t="str">
         <f t="shared" si="0"/>
         <v>name</v>
       </c>
@@ -1400,11 +1416,11 @@
         <v>29</v>
       </c>
       <c r="H31">
-        <f>$A$7</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="J31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K31" t="str">
         <f t="shared" si="0"/>
@@ -1424,7 +1440,7 @@
         <v>7</v>
       </c>
       <c r="J32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K32" t="str">
         <f t="shared" si="0"/>
@@ -1432,17 +1448,21 @@
       </c>
     </row>
     <row r="33" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="G33">
+      <c r="F33" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G33" s="4">
         <v>31</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="4">
         <f>$A$11</f>
         <v>9</v>
       </c>
-      <c r="J33" t="s">
-        <v>51</v>
-      </c>
-      <c r="K33" t="str">
+      <c r="I33" s="4"/>
+      <c r="J33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K33" s="4" t="str">
         <f t="shared" si="0"/>
         <v>message</v>
       </c>
@@ -1452,7 +1472,7 @@
         <v>32</v>
       </c>
       <c r="H34">
-        <f t="shared" ref="H34:H35" si="4">$A$11</f>
+        <f>$A$11</f>
         <v>9</v>
       </c>
       <c r="I34">
@@ -1460,7 +1480,7 @@
         <v>4</v>
       </c>
       <c r="J34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K34" t="str">
         <f t="shared" si="0"/>
@@ -1468,36 +1488,40 @@
       </c>
     </row>
     <row r="35" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="G35">
+      <c r="F35" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G35" s="4">
         <v>33</v>
       </c>
-      <c r="H35">
-        <f t="shared" si="4"/>
+      <c r="H35" s="4">
+        <f>$A$11</f>
         <v>9</v>
       </c>
-      <c r="J35" t="s">
-        <v>52</v>
-      </c>
-      <c r="K35" t="str">
+      <c r="I35" s="4"/>
+      <c r="J35" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K35" s="4" t="str">
         <f t="shared" si="0"/>
         <v>warning</v>
       </c>
     </row>
     <row r="36" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F36" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="G36" s="13">
+      <c r="F36" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G36" s="4">
         <v>34</v>
       </c>
-      <c r="H36" s="13">
+      <c r="H36" s="4">
         <v>10</v>
       </c>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="K36" s="13" t="str">
+      <c r="I36" s="4"/>
+      <c r="J36" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K36" s="4" t="str">
         <f t="shared" si="0"/>
         <v>value</v>
       </c>
@@ -1511,7 +1535,7 @@
         <v>7</v>
       </c>
       <c r="J37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K37" t="str">
         <f t="shared" si="0"/>
@@ -1523,11 +1547,11 @@
         <v>36</v>
       </c>
       <c r="H38">
-        <f t="shared" ref="H38:H40" si="5">$A$9</f>
+        <f>$A$9</f>
         <v>7</v>
       </c>
       <c r="J38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K38" t="str">
         <f t="shared" si="0"/>
@@ -1539,11 +1563,11 @@
         <v>37</v>
       </c>
       <c r="H39">
-        <f t="shared" si="5"/>
+        <f>$A$9</f>
         <v>7</v>
       </c>
       <c r="J39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K39" t="str">
         <f t="shared" si="0"/>
@@ -1555,11 +1579,11 @@
         <v>38</v>
       </c>
       <c r="H40">
-        <f t="shared" si="5"/>
+        <f>$A$9</f>
         <v>7</v>
       </c>
       <c r="J40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K40" t="str">
         <f t="shared" si="0"/>
@@ -1575,10 +1599,10 @@
         <v>1</v>
       </c>
       <c r="J41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="6:11" x14ac:dyDescent="0.25">
@@ -1590,7 +1614,7 @@
         <v>11</v>
       </c>
       <c r="J42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K42" t="str">
         <f>J42</f>

</xml_diff>

<commit_message>
fix BuildAction, SellBuildingAction, UpgradeBuildingAction... add insert and delete for User in UserDbDao add createUser(user), deleteUser(user) in UserDbService
</commit_message>
<xml_diff>
--- a/docs/db_info/monopoly eav.xlsx
+++ b/docs/db_info/monopoly eav.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="61">
   <si>
     <t>OBJTYPE</t>
   </si>
@@ -196,12 +196,6 @@
   </si>
   <si>
     <t>Message</t>
-  </si>
-  <si>
-    <t>---------</t>
-  </si>
-  <si>
-    <t>---</t>
   </si>
   <si>
     <t>extraTurn</t>
@@ -682,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33:F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,7 +977,7 @@
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K8" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1348,17 +1342,18 @@
       </c>
     </row>
     <row r="27" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G27">
+      <c r="G27" s="4">
         <v>25</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="4">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="J27" t="s">
+      <c r="I27" s="4"/>
+      <c r="J27" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="K27" t="str">
+      <c r="K27" s="4" t="str">
         <f t="shared" si="0"/>
         <v>currentPrice</v>
       </c>
@@ -1450,9 +1445,7 @@
       </c>
     </row>
     <row r="33" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F33" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="F33" s="3"/>
       <c r="G33" s="4">
         <v>31</v>
       </c>
@@ -1490,9 +1483,7 @@
       </c>
     </row>
     <row r="35" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F35" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="F35" s="3"/>
       <c r="G35" s="4">
         <v>33</v>
       </c>
@@ -1510,9 +1501,7 @@
       </c>
     </row>
     <row r="36" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F36" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="F36" s="3"/>
       <c r="G36" s="4">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
add PlayerDao.getByParentKey fix pledgedPropertyCheck
</commit_message>
<xml_diff>
--- a/docs/db_info/monopoly eav.xlsx
+++ b/docs/db_info/monopoly eav.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
   <si>
     <t>OBJTYPE</t>
   </si>
@@ -677,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z44"/>
+  <dimension ref="A1:Z43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15:K16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,7 +895,7 @@
         <v>27</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" ref="K5:K42" si="0">J5</f>
+        <f t="shared" ref="K5:K41" si="0">J5</f>
         <v>doublesCount</v>
       </c>
     </row>
@@ -917,7 +917,7 @@
         <v>4</v>
       </c>
       <c r="H6">
-        <f t="shared" ref="H6:H16" si="1">$A$5</f>
+        <f t="shared" ref="H6:H15" si="1">$A$5</f>
         <v>4</v>
       </c>
       <c r="J6" t="s">
@@ -1168,219 +1168,219 @@
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="G16" s="4">
-        <v>42</v>
-      </c>
-      <c r="H16" s="4">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="K16" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>extraTurn</v>
+      <c r="G16">
+        <v>13</v>
+      </c>
+      <c r="H16">
+        <f>$A$6</f>
+        <v>3</v>
+      </c>
+      <c r="J16" t="s">
+        <v>37</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="0"/>
+        <v>basePrice</v>
       </c>
     </row>
     <row r="17" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G17">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H17">
-        <f>$A$6</f>
+        <f t="shared" ref="H17:H26" si="2">$A$6</f>
         <v>3</v>
       </c>
       <c r="J17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K17" t="str">
         <f t="shared" si="0"/>
-        <v>basePrice</v>
+        <v>baseRent</v>
       </c>
     </row>
     <row r="18" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G18">
-        <v>14</v>
-      </c>
-      <c r="H18">
-        <f t="shared" ref="H18:H27" si="2">$A$6</f>
-        <v>3</v>
-      </c>
-      <c r="J18" t="s">
-        <v>38</v>
-      </c>
-      <c r="K18" t="str">
-        <f t="shared" si="0"/>
-        <v>baseRent</v>
-      </c>
-    </row>
-    <row r="19" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G19" s="4">
+      <c r="G18" s="4">
         <v>15</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H18" s="4">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4" t="s">
+      <c r="I18" s="4"/>
+      <c r="J18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="K19" s="4" t="str">
+      <c r="K18" s="4" t="str">
         <f t="shared" si="0"/>
         <v>description</v>
+      </c>
+    </row>
+    <row r="19" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>16</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="J19" t="s">
+        <v>40</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="0"/>
+        <v>maxLevel</v>
       </c>
     </row>
     <row r="20" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G20">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H20">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K20" t="str">
         <f t="shared" si="0"/>
-        <v>maxLevel</v>
+        <v>monopoly</v>
       </c>
     </row>
     <row r="21" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G21">
-        <v>17</v>
-      </c>
-      <c r="H21">
+      <c r="G21" s="4">
+        <v>18</v>
+      </c>
+      <c r="H21" s="4">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J21" t="s">
-        <v>41</v>
-      </c>
-      <c r="K21" t="str">
-        <f t="shared" si="0"/>
-        <v>monopoly</v>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K21" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>name</v>
       </c>
     </row>
     <row r="22" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G22" s="4">
-        <v>18</v>
-      </c>
-      <c r="H22" s="4">
+      <c r="G22">
+        <v>19</v>
+      </c>
+      <c r="H22">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K22" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>name</v>
+      <c r="J22" t="s">
+        <v>42</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="0"/>
+        <v>payBackMoney</v>
       </c>
     </row>
     <row r="23" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G23">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H23">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K23" t="str">
         <f t="shared" si="0"/>
-        <v>payBackMoney</v>
+        <v>pledgePercent</v>
       </c>
     </row>
     <row r="24" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G24">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H24">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J24" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="K24" t="str">
         <f t="shared" si="0"/>
-        <v>pledgePercent</v>
+        <v>position</v>
       </c>
     </row>
     <row r="25" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G25">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H25">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J25" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="K25" t="str">
         <f t="shared" si="0"/>
-        <v>position</v>
+        <v>status</v>
       </c>
     </row>
     <row r="26" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G26">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H26">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J26" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" si="0"/>
-        <v>status</v>
+        <v>turnsToPayBack</v>
       </c>
     </row>
     <row r="27" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G27">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H27">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" ref="H27:H32" si="3">$A$7</f>
+        <v>5</v>
       </c>
       <c r="J27" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K27" t="str">
         <f t="shared" si="0"/>
-        <v>turnsToPayBack</v>
+        <v>currentLevel</v>
       </c>
     </row>
     <row r="28" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G28">
-        <v>24</v>
-      </c>
-      <c r="H28">
-        <f t="shared" ref="H28:H33" si="3">$A$7</f>
+      <c r="G28" s="4">
+        <v>25</v>
+      </c>
+      <c r="H28" s="4">
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="J28" t="s">
-        <v>45</v>
-      </c>
-      <c r="K28" t="str">
-        <f t="shared" si="0"/>
-        <v>currentLevel</v>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K28" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>currentPrice</v>
       </c>
     </row>
     <row r="29" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G29" s="4">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H29" s="4">
         <f t="shared" si="3"/>
@@ -1388,264 +1388,247 @@
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="K29" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>currentPrice</v>
+        <v>description</v>
       </c>
     </row>
     <row r="30" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G30" s="4">
-        <v>26</v>
-      </c>
-      <c r="H30" s="4">
+      <c r="G30">
+        <v>27</v>
+      </c>
+      <c r="H30">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K30" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>description</v>
+      <c r="J30" t="s">
+        <v>40</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="0"/>
+        <v>maxLevel</v>
       </c>
     </row>
     <row r="31" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G31">
-        <v>27</v>
-      </c>
-      <c r="H31">
+      <c r="G31" s="4">
+        <v>28</v>
+      </c>
+      <c r="H31" s="4">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="J31" t="s">
-        <v>40</v>
-      </c>
-      <c r="K31" t="str">
-        <f t="shared" si="0"/>
-        <v>maxLevel</v>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K31" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>name</v>
       </c>
     </row>
     <row r="32" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G32" s="4">
-        <v>28</v>
-      </c>
-      <c r="H32" s="4">
+      <c r="G32">
+        <v>29</v>
+      </c>
+      <c r="H32">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K32" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>name</v>
+      <c r="J32" t="s">
+        <v>47</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="0"/>
+        <v>primaryCost</v>
       </c>
     </row>
     <row r="33" spans="6:11" x14ac:dyDescent="0.25">
       <c r="G33">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H33">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="J33" t="s">
-        <v>47</v>
-      </c>
-      <c r="K33" t="str">
-        <f t="shared" si="0"/>
-        <v>primaryCost</v>
-      </c>
-    </row>
-    <row r="34" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="G34">
-        <v>30</v>
-      </c>
-      <c r="H34">
         <f>$A$10</f>
         <v>8</v>
       </c>
-      <c r="I34">
+      <c r="I33">
         <f>A9</f>
         <v>7</v>
       </c>
-      <c r="J34" t="s">
+      <c r="J33" t="s">
         <v>48</v>
       </c>
-      <c r="K34" t="str">
+      <c r="K33" t="str">
         <f t="shared" si="0"/>
         <v>user_ref</v>
       </c>
     </row>
-    <row r="35" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F35" s="3"/>
-      <c r="G35" s="4">
+    <row r="34" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F34" s="3"/>
+      <c r="G34" s="4">
         <v>31</v>
       </c>
-      <c r="H35" s="4">
+      <c r="H34" s="4">
         <f>$A$11</f>
         <v>9</v>
       </c>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4" t="s">
+      <c r="I34" s="4"/>
+      <c r="J34" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="K35" s="4" t="str">
+      <c r="K34" s="4" t="str">
         <f t="shared" si="0"/>
         <v>message</v>
       </c>
     </row>
-    <row r="36" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="G36">
+    <row r="35" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="G35">
         <v>32</v>
       </c>
-      <c r="H36">
+      <c r="H35">
         <f>$A$11</f>
         <v>9</v>
       </c>
-      <c r="I36">
+      <c r="I35">
         <f>$A$5</f>
         <v>4</v>
       </c>
-      <c r="J36" t="s">
+      <c r="J35" t="s">
         <v>52</v>
       </c>
-      <c r="K36" t="str">
+      <c r="K35" t="str">
         <f t="shared" si="0"/>
         <v>player_ref</v>
+      </c>
+    </row>
+    <row r="36" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F36" s="3"/>
+      <c r="G36" s="4">
+        <v>33</v>
+      </c>
+      <c r="H36" s="4">
+        <f>$A$11</f>
+        <v>9</v>
+      </c>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K36" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>warning</v>
       </c>
     </row>
     <row r="37" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F37" s="3"/>
       <c r="G37" s="4">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H37" s="4">
-        <f>$A$11</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I37" s="4"/>
       <c r="J37" s="4" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="K37" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>warning</v>
+        <v>value</v>
       </c>
     </row>
     <row r="38" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F38" s="3"/>
-      <c r="G38" s="4">
-        <v>34</v>
-      </c>
-      <c r="H38" s="4">
-        <v>10</v>
-      </c>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="K38" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>value</v>
+      <c r="G38">
+        <v>35</v>
+      </c>
+      <c r="H38">
+        <f>$A$9</f>
+        <v>7</v>
+      </c>
+      <c r="J38" t="s">
+        <v>53</v>
+      </c>
+      <c r="K38" t="str">
+        <f t="shared" si="0"/>
+        <v>email</v>
       </c>
     </row>
     <row r="39" spans="6:11" x14ac:dyDescent="0.25">
       <c r="G39">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H39">
         <f>$A$9</f>
         <v>7</v>
       </c>
       <c r="J39" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K39" t="str">
         <f t="shared" si="0"/>
-        <v>email</v>
+        <v>hash</v>
       </c>
     </row>
     <row r="40" spans="6:11" x14ac:dyDescent="0.25">
       <c r="G40">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H40">
         <f>$A$9</f>
         <v>7</v>
       </c>
       <c r="J40" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="K40" t="str">
         <f t="shared" si="0"/>
-        <v>hash</v>
+        <v>name</v>
       </c>
     </row>
     <row r="41" spans="6:11" x14ac:dyDescent="0.25">
       <c r="G41">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H41">
         <f>$A$9</f>
         <v>7</v>
       </c>
       <c r="J41" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="K41" t="str">
         <f t="shared" si="0"/>
-        <v>name</v>
+        <v>password</v>
       </c>
     </row>
     <row r="42" spans="6:11" x14ac:dyDescent="0.25">
       <c r="G42">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H42">
-        <f>$A$9</f>
-        <v>7</v>
+        <f>$A$3</f>
+        <v>1</v>
       </c>
       <c r="J42" t="s">
-        <v>55</v>
-      </c>
-      <c r="K42" t="str">
-        <f t="shared" si="0"/>
-        <v>password</v>
+        <v>56</v>
+      </c>
+      <c r="K42" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="6:11" x14ac:dyDescent="0.25">
       <c r="G43">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H43">
-        <f>$A$3</f>
-        <v>1</v>
-      </c>
-      <c r="J43" t="s">
-        <v>56</v>
-      </c>
-      <c r="K43" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="44" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="G44">
-        <v>40</v>
-      </c>
-      <c r="H44">
         <f>$A$13</f>
         <v>11</v>
       </c>
-      <c r="J44" t="s">
+      <c r="J43" t="s">
         <v>57</v>
       </c>
-      <c r="K44" t="str">
-        <f>J44</f>
+      <c r="K43" t="str">
+        <f>J43</f>
         <v>value</v>
       </c>
     </row>

</xml_diff>